<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@52a5c4bdff10b40fff61f530fa325598604e5851 🚀
</commit_message>
<xml_diff>
--- a/2022/data.xlsx
+++ b/2022/data.xlsx
@@ -2113,7 +2113,7 @@
         <v>5800</v>
       </c>
       <c r="S24" t="n">
-        <v>0</v>
+        <v>72500</v>
       </c>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="b">
@@ -2122,7 +2122,7 @@
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="n">
-        <v>0</v>
+        <v>6041.666666666667</v>
       </c>
     </row>
     <row r="25">
@@ -3350,16 +3350,12 @@
       <c r="R42" t="n">
         <v>4550</v>
       </c>
-      <c r="S42" t="n">
-        <v>56875</v>
-      </c>
+      <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="inlineStr"/>
       <c r="W42" t="inlineStr"/>
-      <c r="X42" t="n">
-        <v>4739.583333333333</v>
-      </c>
+      <c r="X42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -4750,10 +4746,8 @@
       <c r="R62" t="n">
         <v>22500</v>
       </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>350000-400000</t>
-        </is>
+      <c r="S62" t="n">
+        <v>350000</v>
       </c>
       <c r="T62" t="inlineStr">
         <is>
@@ -4765,7 +4759,9 @@
       </c>
       <c r="V62" t="inlineStr"/>
       <c r="W62" t="inlineStr"/>
-      <c r="X62" t="inlineStr"/>
+      <c r="X62" t="n">
+        <v>29166.66666666667</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -9492,18 +9488,14 @@
       <c r="R131" t="n">
         <v>5800</v>
       </c>
-      <c r="S131" t="n">
-        <v>72500</v>
-      </c>
+      <c r="S131" t="inlineStr"/>
       <c r="T131" t="inlineStr"/>
       <c r="U131" t="b">
         <v>1</v>
       </c>
       <c r="V131" t="inlineStr"/>
       <c r="W131" t="inlineStr"/>
-      <c r="X131" t="n">
-        <v>6041.666666666667</v>
-      </c>
+      <c r="X131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
@@ -10888,9 +10880,7 @@
       <c r="R151" t="n">
         <v>7300</v>
       </c>
-      <c r="S151" t="n">
-        <v>91250</v>
-      </c>
+      <c r="S151" t="inlineStr"/>
       <c r="T151" t="inlineStr"/>
       <c r="U151" t="b">
         <v>1</v>
@@ -10905,9 +10895,7 @@
           <t>Tuntilaskutus summaa</t>
         </is>
       </c>
-      <c r="X151" t="n">
-        <v>7604.166666666667</v>
-      </c>
+      <c r="X151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
@@ -12160,10 +12148,8 @@
       <c r="R169" t="n">
         <v>4905</v>
       </c>
-      <c r="S169" t="inlineStr">
-        <is>
-          <t>61312,5</t>
-        </is>
+      <c r="S169" t="n">
+        <v>61312.5</v>
       </c>
       <c r="T169" t="inlineStr"/>
       <c r="U169" t="b">
@@ -12171,7 +12157,9 @@
       </c>
       <c r="V169" t="inlineStr"/>
       <c r="W169" t="inlineStr"/>
-      <c r="X169" t="inlineStr"/>
+      <c r="X169" t="n">
+        <v>5109.375</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
@@ -13537,15 +13525,11 @@
           <t>50/50</t>
         </is>
       </c>
-      <c r="R189" t="inlineStr">
-        <is>
-          <t>4640,71</t>
-        </is>
-      </c>
-      <c r="S189" t="inlineStr">
-        <is>
-          <t>58008,87</t>
-        </is>
+      <c r="R189" t="n">
+        <v>4640.71</v>
+      </c>
+      <c r="S189" t="n">
+        <v>58008.87</v>
       </c>
       <c r="T189" t="inlineStr"/>
       <c r="U189" t="b">
@@ -13553,7 +13537,9 @@
       </c>
       <c r="V189" t="inlineStr"/>
       <c r="W189" t="inlineStr"/>
-      <c r="X189" t="inlineStr"/>
+      <c r="X189" t="n">
+        <v>4834.0725</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
@@ -14295,15 +14281,11 @@
           <t>Toimisto</t>
         </is>
       </c>
-      <c r="R200" t="inlineStr">
-        <is>
-          <t>4239,17</t>
-        </is>
-      </c>
-      <c r="S200" t="inlineStr">
-        <is>
-          <t>60757,96</t>
-        </is>
+      <c r="R200" t="n">
+        <v>4239.17</v>
+      </c>
+      <c r="S200" t="n">
+        <v>60757.96</v>
       </c>
       <c r="T200" t="inlineStr">
         <is>
@@ -14315,7 +14297,9 @@
       </c>
       <c r="V200" t="inlineStr"/>
       <c r="W200" t="inlineStr"/>
-      <c r="X200" t="inlineStr"/>
+      <c r="X200" t="n">
+        <v>5063.163333333333</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="2" t="n">
@@ -14848,9 +14832,7 @@
       <c r="R208" t="n">
         <v>7700</v>
       </c>
-      <c r="S208" t="n">
-        <v>96250</v>
-      </c>
+      <c r="S208" t="inlineStr"/>
       <c r="T208" t="inlineStr"/>
       <c r="U208" t="b">
         <v>1</v>
@@ -14861,9 +14843,7 @@
         </is>
       </c>
       <c r="W208" t="inlineStr"/>
-      <c r="X208" t="n">
-        <v>8020.833333333333</v>
-      </c>
+      <c r="X208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" s="2" t="n">
@@ -16617,15 +16597,11 @@
           <t>50/50</t>
         </is>
       </c>
-      <c r="R234" t="inlineStr">
-        <is>
-          <t>n. 6500</t>
-        </is>
-      </c>
-      <c r="S234" t="inlineStr">
-        <is>
-          <t>n. 81250</t>
-        </is>
+      <c r="R234" t="n">
+        <v>6500</v>
+      </c>
+      <c r="S234" t="n">
+        <v>81250</v>
       </c>
       <c r="T234" t="inlineStr">
         <is>
@@ -16637,7 +16613,9 @@
       </c>
       <c r="V234" t="inlineStr"/>
       <c r="W234" t="inlineStr"/>
-      <c r="X234" t="inlineStr"/>
+      <c r="X234" t="n">
+        <v>6770.833333333333</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="2" t="n">
@@ -17114,18 +17092,14 @@
       <c r="R241" t="n">
         <v>5100</v>
       </c>
-      <c r="S241" t="n">
-        <v>63750</v>
-      </c>
+      <c r="S241" t="inlineStr"/>
       <c r="T241" t="inlineStr"/>
       <c r="U241" t="b">
         <v>1</v>
       </c>
       <c r="V241" t="inlineStr"/>
       <c r="W241" t="inlineStr"/>
-      <c r="X241" t="n">
-        <v>5312.5</v>
-      </c>
+      <c r="X241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" s="2" t="n">
@@ -21050,16 +21024,12 @@
       <c r="R298" t="n">
         <v>6700</v>
       </c>
-      <c r="S298" t="n">
-        <v>83750</v>
-      </c>
+      <c r="S298" t="inlineStr"/>
       <c r="T298" t="inlineStr"/>
       <c r="U298" t="inlineStr"/>
       <c r="V298" t="inlineStr"/>
       <c r="W298" t="inlineStr"/>
-      <c r="X298" t="n">
-        <v>6979.166666666667</v>
-      </c>
+      <c r="X298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" s="2" t="n">
@@ -24610,18 +24580,14 @@
       <c r="R350" t="n">
         <v>4200</v>
       </c>
-      <c r="S350" t="n">
-        <v>52500</v>
-      </c>
+      <c r="S350" t="inlineStr"/>
       <c r="T350" t="inlineStr"/>
       <c r="U350" t="b">
         <v>1</v>
       </c>
       <c r="V350" t="inlineStr"/>
       <c r="W350" t="inlineStr"/>
-      <c r="X350" t="n">
-        <v>4375</v>
-      </c>
+      <c r="X350" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" s="2" t="n">
@@ -26480,18 +26446,14 @@
       <c r="R378" t="n">
         <v>4500</v>
       </c>
-      <c r="S378" t="n">
-        <v>56250</v>
-      </c>
+      <c r="S378" t="inlineStr"/>
       <c r="T378" t="inlineStr"/>
       <c r="U378" t="b">
         <v>0</v>
       </c>
       <c r="V378" t="inlineStr"/>
       <c r="W378" t="inlineStr"/>
-      <c r="X378" t="n">
-        <v>4687.5</v>
-      </c>
+      <c r="X378" t="inlineStr"/>
     </row>
     <row r="379">
       <c r="A379" s="2" t="n">
@@ -28192,10 +28154,8 @@
       <c r="R403" t="n">
         <v>4500</v>
       </c>
-      <c r="S403" t="inlineStr">
-        <is>
-          <t>56, 250</t>
-        </is>
+      <c r="S403" t="n">
+        <v>56250</v>
       </c>
       <c r="T403" t="inlineStr"/>
       <c r="U403" t="b">
@@ -28203,7 +28163,9 @@
       </c>
       <c r="V403" t="inlineStr"/>
       <c r="W403" t="inlineStr"/>
-      <c r="X403" t="inlineStr"/>
+      <c r="X403" t="n">
+        <v>4687.5</v>
+      </c>
     </row>
     <row r="404">
       <c r="A404" s="2" t="n">
@@ -29133,10 +29095,8 @@
           <t>50/50</t>
         </is>
       </c>
-      <c r="R417" t="inlineStr">
-        <is>
-          <t>5259,29</t>
-        </is>
+      <c r="R417" t="n">
+        <v>5259.29</v>
       </c>
       <c r="S417" t="n">
         <v>65741</v>
@@ -29696,18 +29656,14 @@
       <c r="R425" t="n">
         <v>6300</v>
       </c>
-      <c r="S425" t="n">
-        <v>78750</v>
-      </c>
+      <c r="S425" t="inlineStr"/>
       <c r="T425" t="inlineStr"/>
       <c r="U425" t="b">
         <v>1</v>
       </c>
       <c r="V425" t="inlineStr"/>
       <c r="W425" t="inlineStr"/>
-      <c r="X425" t="n">
-        <v>6562.5</v>
-      </c>
+      <c r="X425" t="inlineStr"/>
     </row>
     <row r="426">
       <c r="A426" s="2" t="n">
@@ -32084,10 +32040,8 @@
       <c r="R459" t="n">
         <v>6100</v>
       </c>
-      <c r="S459" t="inlineStr">
-        <is>
-          <t>n. 100 000€</t>
-        </is>
+      <c r="S459" t="n">
+        <v>100000</v>
       </c>
       <c r="T459" t="inlineStr">
         <is>
@@ -32099,7 +32053,9 @@
       </c>
       <c r="V459" t="inlineStr"/>
       <c r="W459" t="inlineStr"/>
-      <c r="X459" t="inlineStr"/>
+      <c r="X459" t="n">
+        <v>8333.333333333334</v>
+      </c>
     </row>
     <row r="460">
       <c r="A460" s="2" t="n">
@@ -34516,10 +34472,8 @@
       <c r="R494" t="n">
         <v>9000</v>
       </c>
-      <c r="S494" t="inlineStr">
-        <is>
-          <t>112,5</t>
-        </is>
+      <c r="S494" t="n">
+        <v>112500</v>
       </c>
       <c r="T494" t="inlineStr"/>
       <c r="U494" t="b">
@@ -34527,7 +34481,9 @@
       </c>
       <c r="V494" t="inlineStr"/>
       <c r="W494" t="inlineStr"/>
-      <c r="X494" t="inlineStr"/>
+      <c r="X494" t="n">
+        <v>9375</v>
+      </c>
     </row>
     <row r="495">
       <c r="A495" s="2" t="n">
@@ -35506,18 +35462,14 @@
       <c r="R508" t="n">
         <v>3350</v>
       </c>
-      <c r="S508" t="n">
-        <v>41875</v>
-      </c>
+      <c r="S508" t="inlineStr"/>
       <c r="T508" t="inlineStr"/>
       <c r="U508" t="b">
         <v>0</v>
       </c>
       <c r="V508" t="inlineStr"/>
       <c r="W508" t="inlineStr"/>
-      <c r="X508" t="n">
-        <v>3489.583333333333</v>
-      </c>
+      <c r="X508" t="inlineStr"/>
     </row>
     <row r="509">
       <c r="A509" s="2" t="n">
@@ -36194,9 +36146,7 @@
       <c r="R518" t="n">
         <v>4500</v>
       </c>
-      <c r="S518" t="n">
-        <v>56250</v>
-      </c>
+      <c r="S518" t="inlineStr"/>
       <c r="T518" t="n">
         <v>56000</v>
       </c>
@@ -36205,9 +36155,7 @@
       </c>
       <c r="V518" t="inlineStr"/>
       <c r="W518" t="inlineStr"/>
-      <c r="X518" t="n">
-        <v>4687.5</v>
-      </c>
+      <c r="X518" t="inlineStr"/>
     </row>
     <row r="519">
       <c r="A519" s="2" t="n">
@@ -36472,18 +36420,14 @@
       <c r="R522" t="n">
         <v>4000</v>
       </c>
-      <c r="S522" t="n">
-        <v>50000</v>
-      </c>
+      <c r="S522" t="inlineStr"/>
       <c r="T522" t="inlineStr"/>
       <c r="U522" t="b">
         <v>1</v>
       </c>
       <c r="V522" t="inlineStr"/>
       <c r="W522" t="inlineStr"/>
-      <c r="X522" t="n">
-        <v>4166.666666666667</v>
-      </c>
+      <c r="X522" t="inlineStr"/>
     </row>
     <row r="523">
       <c r="A523" s="2" t="n">
@@ -37500,18 +37444,14 @@
       <c r="R537" t="n">
         <v>6500</v>
       </c>
-      <c r="S537" t="n">
-        <v>81250</v>
-      </c>
+      <c r="S537" t="inlineStr"/>
       <c r="T537" t="inlineStr"/>
       <c r="U537" t="b">
         <v>1</v>
       </c>
       <c r="V537" t="inlineStr"/>
       <c r="W537" t="inlineStr"/>
-      <c r="X537" t="n">
-        <v>6770.833333333333</v>
-      </c>
+      <c r="X537" t="inlineStr"/>
     </row>
     <row r="538">
       <c r="A538" s="2" t="n">
@@ -37916,18 +37856,14 @@
       <c r="R543" t="n">
         <v>6000</v>
       </c>
-      <c r="S543" t="n">
-        <v>75000</v>
-      </c>
+      <c r="S543" t="inlineStr"/>
       <c r="T543" t="inlineStr"/>
       <c r="U543" t="b">
         <v>1</v>
       </c>
       <c r="V543" t="inlineStr"/>
       <c r="W543" t="inlineStr"/>
-      <c r="X543" t="n">
-        <v>6250</v>
-      </c>
+      <c r="X543" t="inlineStr"/>
     </row>
     <row r="544">
       <c r="A544" s="2" t="n">
@@ -40919,10 +40855,8 @@
       <c r="R587" t="n">
         <v>5145</v>
       </c>
-      <c r="S587" t="inlineStr">
-        <is>
-          <t>64 312,5</t>
-        </is>
+      <c r="S587" t="n">
+        <v>64312.5</v>
       </c>
       <c r="T587" t="inlineStr">
         <is>
@@ -40934,7 +40868,9 @@
       </c>
       <c r="V587" t="inlineStr"/>
       <c r="W587" t="inlineStr"/>
-      <c r="X587" t="inlineStr"/>
+      <c r="X587" t="n">
+        <v>5359.375</v>
+      </c>
     </row>
     <row r="588">
       <c r="A588" s="2" t="n">
@@ -42401,18 +42337,14 @@
       <c r="R609" t="n">
         <v>5100</v>
       </c>
-      <c r="S609" t="n">
-        <v>63750</v>
-      </c>
+      <c r="S609" t="inlineStr"/>
       <c r="T609" t="inlineStr"/>
       <c r="U609" t="b">
         <v>1</v>
       </c>
       <c r="V609" t="inlineStr"/>
       <c r="W609" t="inlineStr"/>
-      <c r="X609" t="n">
-        <v>5312.5</v>
-      </c>
+      <c r="X609" t="inlineStr"/>
     </row>
     <row r="610">
       <c r="A610" s="2" t="n">
@@ -42803,18 +42735,14 @@
       <c r="R615" t="n">
         <v>2800</v>
       </c>
-      <c r="S615" t="n">
-        <v>35000</v>
-      </c>
+      <c r="S615" t="inlineStr"/>
       <c r="T615" t="inlineStr"/>
       <c r="U615" t="b">
         <v>0</v>
       </c>
       <c r="V615" t="inlineStr"/>
       <c r="W615" t="inlineStr"/>
-      <c r="X615" t="n">
-        <v>2916.666666666667</v>
-      </c>
+      <c r="X615" t="inlineStr"/>
     </row>
     <row r="616">
       <c r="A616" s="2" t="n">
@@ -44012,9 +43940,7 @@
       <c r="R632" t="n">
         <v>3990</v>
       </c>
-      <c r="S632" t="n">
-        <v>49875</v>
-      </c>
+      <c r="S632" t="inlineStr"/>
       <c r="T632" t="inlineStr"/>
       <c r="U632" t="b">
         <v>0</v>
@@ -44029,9 +43955,7 @@
           <t>mietityttää, olisiko kuitenkin koulutustausta relevantti tieto?</t>
         </is>
       </c>
-      <c r="X632" t="n">
-        <v>4156.25</v>
-      </c>
+      <c r="X632" t="inlineStr"/>
     </row>
     <row r="633">
       <c r="A633" s="2" t="n">
@@ -44084,10 +44008,8 @@
       <c r="R633" t="n">
         <v>5565</v>
       </c>
-      <c r="S633" t="inlineStr">
-        <is>
-          <t>69562,5</t>
-        </is>
+      <c r="S633" t="n">
+        <v>69562.5</v>
       </c>
       <c r="T633" t="inlineStr">
         <is>
@@ -44099,7 +44021,9 @@
       </c>
       <c r="V633" t="inlineStr"/>
       <c r="W633" t="inlineStr"/>
-      <c r="X633" t="inlineStr"/>
+      <c r="X633" t="n">
+        <v>5796.875</v>
+      </c>
     </row>
     <row r="634">
       <c r="A634" s="2" t="n">
@@ -44513,7 +44437,7 @@
         <v>5000</v>
       </c>
       <c r="S639" t="n">
-        <v>62.5</v>
+        <v>62500</v>
       </c>
       <c r="T639" t="inlineStr"/>
       <c r="U639" t="b">
@@ -44522,7 +44446,7 @@
       <c r="V639" t="inlineStr"/>
       <c r="W639" t="inlineStr"/>
       <c r="X639" t="n">
-        <v>5.208333333333333</v>
+        <v>5208.333333333333</v>
       </c>
     </row>
     <row r="640">
@@ -44716,18 +44640,14 @@
       <c r="R642" t="n">
         <v>3190</v>
       </c>
-      <c r="S642" t="n">
-        <v>39875</v>
-      </c>
+      <c r="S642" t="inlineStr"/>
       <c r="T642" t="inlineStr"/>
       <c r="U642" t="b">
         <v>0</v>
       </c>
       <c r="V642" t="inlineStr"/>
       <c r="W642" t="inlineStr"/>
-      <c r="X642" t="n">
-        <v>3322.916666666667</v>
-      </c>
+      <c r="X642" t="inlineStr"/>
     </row>
     <row r="643">
       <c r="A643" s="2" t="n">
@@ -46006,9 +45926,7 @@
       <c r="R661" t="n">
         <v>7300</v>
       </c>
-      <c r="S661" t="n">
-        <v>91250</v>
-      </c>
+      <c r="S661" t="inlineStr"/>
       <c r="T661" t="n">
         <v>91250</v>
       </c>
@@ -46017,9 +45935,7 @@
       </c>
       <c r="V661" t="inlineStr"/>
       <c r="W661" t="inlineStr"/>
-      <c r="X661" t="n">
-        <v>7604.166666666667</v>
-      </c>
+      <c r="X661" t="inlineStr"/>
     </row>
     <row r="662">
       <c r="A662" s="2" t="n">
@@ -46148,9 +46064,7 @@
       <c r="R663" t="n">
         <v>3000</v>
       </c>
-      <c r="S663" t="n">
-        <v>37500</v>
-      </c>
+      <c r="S663" t="inlineStr"/>
       <c r="T663" t="inlineStr"/>
       <c r="U663" t="b">
         <v>1</v>
@@ -46161,9 +46075,7 @@
         </is>
       </c>
       <c r="W663" t="inlineStr"/>
-      <c r="X663" t="n">
-        <v>3125</v>
-      </c>
+      <c r="X663" t="inlineStr"/>
     </row>
     <row r="664">
       <c r="A664" s="2" t="n">
@@ -47298,18 +47210,14 @@
       <c r="R680" t="n">
         <v>5100</v>
       </c>
-      <c r="S680" t="n">
-        <v>63750</v>
-      </c>
+      <c r="S680" t="inlineStr"/>
       <c r="T680" t="inlineStr"/>
       <c r="U680" t="b">
         <v>0</v>
       </c>
       <c r="V680" t="inlineStr"/>
       <c r="W680" t="inlineStr"/>
-      <c r="X680" t="n">
-        <v>5312.5</v>
-      </c>
+      <c r="X680" t="inlineStr"/>
     </row>
     <row r="681">
       <c r="A681" s="2" t="n">

</xml_diff>